<commit_message>
Add missing files Fix tests based on PR review comments
</commit_message>
<xml_diff>
--- a/test/core/excel/ReadOnlyFile.xlsx
+++ b/test/core/excel/ReadOnlyFile.xlsx
@@ -21,17 +21,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>word</t>
-  </si>
-  <si>
-    <t>palabra</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -347,7 +336,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
@@ -357,27 +346,37 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
+      <c r="A2">
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>1</v>
+      <c r="A5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>